<commit_message>
Writing SE tables for CLL, MDS, and MM.
</commit_message>
<xml_diff>
--- a/tables/CNV_TFPN_cnvkit_region.xlsx
+++ b/tables/CNV_TFPN_cnvkit_region.xlsx
@@ -522,10 +522,10 @@
   <dimension ref="A1:BJ201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1503,7 +1503,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SLL</t>
+          <t>CLL</t>
         </is>
       </c>
       <c r="B5" s="14" t="inlineStr">
@@ -4243,7 +4243,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CLL/MZL/LPL</t>
+          <t>CLL</t>
         </is>
       </c>
       <c r="B18" s="14" t="inlineStr">
@@ -4876,7 +4876,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SLL</t>
+          <t>CLL</t>
         </is>
       </c>
       <c r="B21" s="14" t="inlineStr">
@@ -7386,7 +7386,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MF, CD5+ small B cell lymphoproliferative</t>
+          <t>CLL</t>
         </is>
       </c>
       <c r="B33" s="18" t="inlineStr">
@@ -10534,7 +10534,7 @@
     <row r="48">
       <c r="A48" s="20" t="inlineStr">
         <is>
-          <t>MDS s/p allogeneic bone marrow transplant</t>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B48" s="18" t="inlineStr">
@@ -10749,7 +10749,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -10965,9 +10965,9 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>MDS therapy related</t>
+      <c r="A50" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B50" s="18" t="inlineStr">
@@ -11181,7 +11181,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -11397,7 +11397,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -11613,7 +11613,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -11829,7 +11829,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -12045,7 +12045,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -12261,7 +12261,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -12477,9 +12477,9 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>MDS isolated del(5q)</t>
+      <c r="A57" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B57" s="18" t="inlineStr">
@@ -12688,9 +12688,9 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>MDS isolated del(5q)</t>
+      <c r="A58" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B58" s="18" t="inlineStr">
@@ -12904,9 +12904,9 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>MDS, Refractory cytopenia with unilineage dysplasia</t>
+      <c r="A59" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B59" s="18" t="inlineStr">
@@ -13120,7 +13120,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -13336,7 +13336,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -13552,7 +13552,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -13773,9 +13773,9 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>MDS-EB-1</t>
+      <c r="A63" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B63" s="18" t="inlineStr">
@@ -13989,9 +13989,9 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>MDS therapy related</t>
+      <c r="A64" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B64" s="18" t="inlineStr">
@@ -14205,9 +14205,9 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>MDS, Refractory anemia with excess blasts</t>
+      <c r="A65" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B65" s="18" t="inlineStr">
@@ -14421,7 +14421,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -14637,9 +14637,9 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>MDS, Refractory cytopenia with multilineage dysplasia</t>
+      <c r="A67" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B67" s="18" t="inlineStr">
@@ -14853,9 +14853,9 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>MDS with multilineage dysplasia</t>
+      <c r="A68" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B68" s="18" t="inlineStr">
@@ -15069,9 +15069,9 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>MDS, Refractory anemia with excess blasts</t>
+      <c r="A69" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B69" s="18" t="inlineStr">
@@ -15285,7 +15285,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -15501,7 +15501,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -15713,9 +15713,9 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>MDS therapy related</t>
+      <c r="A72" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B72" s="18" t="inlineStr">
@@ -15929,9 +15929,9 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>MDS/MPN, CMML</t>
+      <c r="A73" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B73" s="18" t="inlineStr">
@@ -16145,7 +16145,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -16361,7 +16361,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="A75" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -16577,7 +16577,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
+      <c r="A76" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -16793,7 +16793,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
+      <c r="A77" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -17009,7 +17009,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -17225,9 +17225,9 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MDS/MPN </t>
+      <c r="A79" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B79" s="18" t="inlineStr">
@@ -17441,7 +17441,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
+      <c r="A80" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -17662,7 +17662,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
+      <c r="A81" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -17878,7 +17878,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
+      <c r="A82" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -18094,7 +18094,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
+      <c r="A83" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -18310,7 +18310,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
+      <c r="A84" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -18526,7 +18526,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
+      <c r="A85" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -18742,7 +18742,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
+      <c r="A86" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -18954,7 +18954,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
+      <c r="A87" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -19165,7 +19165,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
+      <c r="A88" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -19381,7 +19381,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="A89" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -19597,7 +19597,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
+      <c r="A90" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -19813,9 +19813,9 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>MDS isolated del(5q)</t>
+      <c r="A91" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B91" s="18" t="inlineStr">
@@ -20024,9 +20024,9 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>MDS, Refractory anemia with ring sideroblasts</t>
+      <c r="A92" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B92" s="18" t="inlineStr">
@@ -20240,7 +20240,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
+      <c r="A93" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -20456,7 +20456,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
+      <c r="A94" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -20672,9 +20672,9 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>MDS/MPN, CMML</t>
+      <c r="A95" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B95" s="18" t="inlineStr">
@@ -20888,9 +20888,9 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>MDS-EB</t>
+      <c r="A96" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B96" s="18" t="inlineStr">
@@ -21099,9 +21099,9 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>MDS with multilineage dysplasia and myelofibrosis</t>
+      <c r="A97" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B97" s="18" t="inlineStr">
@@ -21315,7 +21315,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
+      <c r="A98" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -21531,9 +21531,9 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>MDS-EB</t>
+      <c r="A99" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B99" s="18" t="inlineStr">
@@ -21747,7 +21747,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
+      <c r="A100" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -21963,9 +21963,9 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>MDS/MPN, CMML</t>
+      <c r="A101" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B101" s="18" t="inlineStr">
@@ -22179,9 +22179,9 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>MDS isolated del(5q)</t>
+      <c r="A102" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B102" s="18" t="inlineStr">
@@ -22395,7 +22395,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
+      <c r="A103" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -22611,7 +22611,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
+      <c r="A104" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -22827,9 +22827,9 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>MDS,  Refractory anemia with ring sideroblasts</t>
+      <c r="A105" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B105" s="18" t="inlineStr">
@@ -23048,7 +23048,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
+      <c r="A106" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -23264,9 +23264,9 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>MDS-EB2</t>
+      <c r="A107" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B107" s="18" t="inlineStr">
@@ -23485,9 +23485,9 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>MDS-EB2</t>
+      <c r="A108" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B108" s="18" t="inlineStr">
@@ -23706,9 +23706,9 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>MDS, Refractory anemia with excess blasts</t>
+      <c r="A109" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B109" s="18" t="inlineStr">
@@ -23922,7 +23922,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
+      <c r="A110" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -24138,9 +24138,9 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>MDS, Refractory cytopenia with multilineage dysplasia</t>
+      <c r="A111" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B111" s="18" t="inlineStr">
@@ -24354,9 +24354,9 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>MDS, Refractory cytopenia with multilineage dysplasia</t>
+      <c r="A112" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B112" s="18" t="inlineStr">
@@ -24570,7 +24570,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
+      <c r="A113" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -24786,9 +24786,9 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>MDS/MPN</t>
+      <c r="A114" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B114" s="18" t="inlineStr">
@@ -25002,9 +25002,9 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>MDS, Refractory cytopenia with multilineage dysplasia</t>
+      <c r="A115" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B115" s="18" t="inlineStr">
@@ -25213,7 +25213,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
+      <c r="A116" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -25429,7 +25429,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
+      <c r="A117" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -25645,7 +25645,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
+      <c r="A118" s="20" t="inlineStr">
         <is>
           <t>MDS</t>
         </is>
@@ -25861,9 +25861,9 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>MDS + CML</t>
+      <c r="A119" s="20" t="inlineStr">
+        <is>
+          <t>MDS</t>
         </is>
       </c>
       <c r="B119" s="18" t="inlineStr">

</xml_diff>

<commit_message>
Correct generateplotsSE.py script in tables directory.
Storing tableSE figures.
</commit_message>
<xml_diff>
--- a/tables/CNV_TFPN_cnvkit_region.xlsx
+++ b/tables/CNV_TFPN_cnvkit_region.xlsx
@@ -1262,7 +1262,7 @@
       </c>
       <c r="AZ3" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA3" s="20" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="AV5" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW5" s="20" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="AR6" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS6" s="20" t="inlineStr">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="AV7" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW7" s="20" t="inlineStr">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="AZ9" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA9" s="20" t="inlineStr">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="AZ10" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA10" s="20" t="inlineStr">
@@ -2949,7 +2949,7 @@
       </c>
       <c r="AZ11" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA11" s="20" t="inlineStr">
@@ -3122,7 +3122,7 @@
       </c>
       <c r="AR12" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS12" s="20" t="inlineStr">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="AV12" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AW12" s="20" t="inlineStr">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="AQ13" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR13" s="20" t="inlineStr">
@@ -3757,7 +3757,7 @@
       </c>
       <c r="AR15" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS15" s="20" t="inlineStr">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="AV17" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW17" s="20" t="inlineStr">
@@ -4597,7 +4597,7 @@
       </c>
       <c r="AR19" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS19" s="20" t="inlineStr">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="AZ20" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA20" s="20" t="inlineStr">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="AR22" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS22" s="20" t="inlineStr">
@@ -5437,7 +5437,7 @@
       </c>
       <c r="AQ23" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR23" s="20" t="inlineStr">
@@ -5653,7 +5653,7 @@
       </c>
       <c r="AR24" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS24" s="20" t="inlineStr">
@@ -5691,7 +5691,7 @@
       </c>
       <c r="AZ24" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA24" s="20" t="inlineStr">
@@ -7102,7 +7102,7 @@
       </c>
       <c r="AQ31" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AR31" s="20" t="inlineStr">
@@ -7127,7 +7127,7 @@
       </c>
       <c r="AV31" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW31" s="20" t="inlineStr">
@@ -7313,12 +7313,12 @@
       </c>
       <c r="AQ32" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR32" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS32" s="20" t="inlineStr">
@@ -7520,7 +7520,7 @@
       </c>
       <c r="AQ33" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AR33" s="20" t="inlineStr">
@@ -8366,7 +8366,7 @@
       </c>
       <c r="AQ37" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AR37" s="20" t="inlineStr">
@@ -8409,7 +8409,7 @@
       </c>
       <c r="AZ37" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA37" s="20" t="inlineStr">
@@ -8992,7 +8992,7 @@
       </c>
       <c r="AR40" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS40" s="20" t="inlineStr">
@@ -9198,7 +9198,7 @@
       </c>
       <c r="AQ41" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR41" s="20" t="inlineStr">
@@ -9415,7 +9415,7 @@
       </c>
       <c r="AR42" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS42" s="20" t="inlineStr">
@@ -9626,7 +9626,7 @@
       </c>
       <c r="AR43" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS43" s="20" t="inlineStr">
@@ -9646,7 +9646,7 @@
       </c>
       <c r="AV43" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW43" s="20" t="inlineStr">
@@ -9837,7 +9837,7 @@
       </c>
       <c r="AR44" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS44" s="20" t="inlineStr">
@@ -10715,7 +10715,7 @@
       </c>
       <c r="AZ48" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA48" s="20" t="inlineStr">
@@ -11580,7 +11580,7 @@
       </c>
       <c r="AZ52" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA52" s="20" t="inlineStr">
@@ -11796,7 +11796,7 @@
       </c>
       <c r="AZ53" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA53" s="20" t="inlineStr">
@@ -12012,7 +12012,7 @@
       </c>
       <c r="AZ54" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA54" s="20" t="inlineStr">
@@ -12444,7 +12444,7 @@
       </c>
       <c r="AZ56" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA56" s="20" t="inlineStr">
@@ -12871,7 +12871,7 @@
       </c>
       <c r="AZ58" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA58" s="20" t="inlineStr">
@@ -13717,7 +13717,7 @@
       </c>
       <c r="AV62" s="20" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="AW62" s="20" t="inlineStr">
@@ -13918,7 +13918,7 @@
       </c>
       <c r="AR63" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS63" s="20" t="inlineStr">
@@ -14172,7 +14172,7 @@
       </c>
       <c r="AZ64" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA64" s="20" t="inlineStr">
@@ -15662,7 +15662,7 @@
       </c>
       <c r="AV71" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW71" s="20" t="inlineStr">
@@ -15858,7 +15858,7 @@
       </c>
       <c r="AR72" s="20" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="AS72" s="20" t="inlineStr">
@@ -16094,7 +16094,7 @@
       </c>
       <c r="AV73" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW73" s="20" t="inlineStr">
@@ -16328,7 +16328,7 @@
       </c>
       <c r="AZ74" s="20" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="BA74" s="20" t="inlineStr">
@@ -16506,7 +16506,7 @@
       </c>
       <c r="AR75" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS75" s="20" t="inlineStr">
@@ -16544,7 +16544,7 @@
       </c>
       <c r="AZ75" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA75" s="20" t="inlineStr">
@@ -16760,7 +16760,7 @@
       </c>
       <c r="AZ76" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA76" s="20" t="inlineStr">
@@ -17154,7 +17154,7 @@
       </c>
       <c r="AR78" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS78" s="20" t="inlineStr">
@@ -17174,7 +17174,7 @@
       </c>
       <c r="AV78" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW78" s="20" t="inlineStr">
@@ -17365,7 +17365,7 @@
       </c>
       <c r="AQ79" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR79" s="20" t="inlineStr">
@@ -17624,7 +17624,7 @@
       </c>
       <c r="AZ80" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA80" s="20" t="inlineStr">
@@ -18878,7 +18878,7 @@
       </c>
       <c r="AQ86" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AR86" s="20" t="inlineStr">
@@ -19119,7 +19119,7 @@
       </c>
       <c r="AV87" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW87" s="20" t="inlineStr">
@@ -19305,7 +19305,7 @@
       </c>
       <c r="AQ88" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR88" s="20" t="inlineStr">
@@ -20164,7 +20164,7 @@
       </c>
       <c r="AQ92" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR92" s="20" t="inlineStr">
@@ -20189,7 +20189,7 @@
       </c>
       <c r="AV92" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW92" s="20" t="inlineStr">
@@ -21244,7 +21244,7 @@
       </c>
       <c r="AR97" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS97" s="20" t="inlineStr">
@@ -21480,7 +21480,7 @@
       </c>
       <c r="AV98" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW98" s="20" t="inlineStr">
@@ -21498,7 +21498,7 @@
       </c>
       <c r="AZ98" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA98" s="20" t="inlineStr">
@@ -21912,7 +21912,7 @@
       </c>
       <c r="AV100" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW100" s="20" t="inlineStr">
@@ -22324,7 +22324,7 @@
       </c>
       <c r="AR102" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS102" s="20" t="inlineStr">
@@ -22344,7 +22344,7 @@
       </c>
       <c r="AV102" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW102" s="20" t="inlineStr">
@@ -22578,7 +22578,7 @@
       </c>
       <c r="AZ103" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA103" s="20" t="inlineStr">
@@ -22972,7 +22972,7 @@
       </c>
       <c r="AR105" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS105" s="20" t="inlineStr">
@@ -23188,7 +23188,7 @@
       </c>
       <c r="AQ106" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR106" s="20" t="inlineStr">
@@ -23231,7 +23231,7 @@
       </c>
       <c r="AZ106" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA106" s="20" t="inlineStr">
@@ -23409,7 +23409,7 @@
       </c>
       <c r="AR107" s="20" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="AS107" s="20" t="inlineStr">
@@ -23630,7 +23630,7 @@
       </c>
       <c r="AR108" s="20" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="AS108" s="20" t="inlineStr">
@@ -24537,7 +24537,7 @@
       </c>
       <c r="AZ112" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA112" s="20" t="inlineStr">
@@ -24926,7 +24926,7 @@
       </c>
       <c r="AQ114" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR114" s="20" t="inlineStr">
@@ -25185,7 +25185,7 @@
       </c>
       <c r="AZ115" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA115" s="20" t="inlineStr">
@@ -25353,7 +25353,7 @@
       </c>
       <c r="AQ116" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR116" s="20" t="inlineStr">
@@ -26236,7 +26236,7 @@
       </c>
       <c r="AV120" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AW120" s="20" t="inlineStr">
@@ -26254,7 +26254,7 @@
       </c>
       <c r="AZ120" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA120" s="20" t="inlineStr">
@@ -26465,7 +26465,7 @@
       </c>
       <c r="AZ121" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA121" s="20" t="inlineStr">
@@ -27108,7 +27108,7 @@
       </c>
       <c r="AZ124" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA124" s="20" t="inlineStr">
@@ -27286,7 +27286,7 @@
       </c>
       <c r="AQ125" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AR125" s="20" t="inlineStr">
@@ -27502,7 +27502,7 @@
       </c>
       <c r="AR126" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS126" s="20" t="inlineStr">
@@ -28145,7 +28145,7 @@
       </c>
       <c r="AR129" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS129" s="20" t="inlineStr">
@@ -28165,7 +28165,7 @@
       </c>
       <c r="AV129" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW129" s="20" t="inlineStr">
@@ -28183,7 +28183,7 @@
       </c>
       <c r="AZ129" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA129" s="20" t="inlineStr">
@@ -28356,7 +28356,7 @@
       </c>
       <c r="AR130" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS130" s="20" t="inlineStr">
@@ -28376,7 +28376,7 @@
       </c>
       <c r="AV130" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW130" s="20" t="inlineStr">
@@ -28778,7 +28778,7 @@
       </c>
       <c r="AR132" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS132" s="20" t="inlineStr">
@@ -28981,7 +28981,7 @@
       </c>
       <c r="AQ133" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR133" s="20" t="inlineStr">
@@ -29024,7 +29024,7 @@
       </c>
       <c r="AZ133" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA133" s="20" t="inlineStr">
@@ -29428,7 +29428,7 @@
       </c>
       <c r="AV135" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW135" s="20" t="inlineStr">
@@ -29446,7 +29446,7 @@
       </c>
       <c r="AZ135" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA135" s="20" t="inlineStr">
@@ -29624,7 +29624,7 @@
       </c>
       <c r="AR136" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS136" s="20" t="inlineStr">
@@ -29662,7 +29662,7 @@
       </c>
       <c r="AZ136" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA136" s="20" t="inlineStr">
@@ -29840,7 +29840,7 @@
       </c>
       <c r="AR137" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS137" s="20" t="inlineStr">
@@ -29860,7 +29860,7 @@
       </c>
       <c r="AV137" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW137" s="20" t="inlineStr">
@@ -30282,7 +30282,7 @@
       </c>
       <c r="AV139" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW139" s="20" t="inlineStr">
@@ -30300,7 +30300,7 @@
       </c>
       <c r="AZ139" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA139" s="20" t="inlineStr">
@@ -30684,12 +30684,12 @@
       </c>
       <c r="AQ141" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR141" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS141" s="20" t="inlineStr">
@@ -31114,7 +31114,7 @@
       </c>
       <c r="AR143" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS143" s="20" t="inlineStr">
@@ -31152,7 +31152,7 @@
       </c>
       <c r="AZ143" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA143" s="20" t="inlineStr">
@@ -31729,7 +31729,7 @@
       </c>
       <c r="AR146" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS146" s="20" t="inlineStr">
@@ -32350,7 +32350,7 @@
       </c>
       <c r="AR149" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS149" s="20" t="inlineStr">
@@ -32968,7 +32968,7 @@
       </c>
       <c r="AQ152" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR152" s="20" t="inlineStr">
@@ -33011,7 +33011,7 @@
       </c>
       <c r="AZ152" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="BA152" s="20" t="inlineStr">
@@ -33394,7 +33394,7 @@
       </c>
       <c r="AR154" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS154" s="20" t="inlineStr">
@@ -33600,7 +33600,7 @@
       </c>
       <c r="AQ155" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR155" s="20" t="inlineStr">
@@ -33836,7 +33836,7 @@
       </c>
       <c r="AV156" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW156" s="20" t="inlineStr">
@@ -34027,7 +34027,7 @@
       </c>
       <c r="AR157" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS157" s="20" t="inlineStr">
@@ -35303,7 +35303,7 @@
       </c>
       <c r="AV163" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW163" s="20" t="inlineStr">
@@ -35532,7 +35532,7 @@
       </c>
       <c r="AZ164" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA164" s="20" t="inlineStr">
@@ -35695,7 +35695,7 @@
       </c>
       <c r="AQ165" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR165" s="20" t="inlineStr">
@@ -36333,7 +36333,7 @@
       </c>
       <c r="AR168" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS168" s="20" t="inlineStr">
@@ -36353,7 +36353,7 @@
       </c>
       <c r="AV168" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW168" s="20" t="inlineStr">
@@ -36581,7 +36581,7 @@
       </c>
       <c r="AZ169" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA169" s="20" t="inlineStr">
@@ -36792,7 +36792,7 @@
       </c>
       <c r="AZ170" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA170" s="20" t="inlineStr">
@@ -37191,7 +37191,7 @@
       </c>
       <c r="AV172" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW172" s="20" t="inlineStr">
@@ -37626,7 +37626,7 @@
       </c>
       <c r="AZ174" s="20" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="BA174" s="20" t="inlineStr">
@@ -38205,7 +38205,7 @@
       </c>
       <c r="AR177" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS177" s="20" t="inlineStr">
@@ -38460,7 +38460,7 @@
       </c>
       <c r="AZ178" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA178" s="20" t="inlineStr">
@@ -38682,7 +38682,7 @@
       </c>
       <c r="AZ179" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA179" s="20" t="inlineStr">
@@ -39068,7 +39068,7 @@
       </c>
       <c r="AR181" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS181" s="20" t="inlineStr">
@@ -39275,7 +39275,7 @@
       </c>
       <c r="AQ182" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR182" s="20" t="inlineStr">
@@ -39729,7 +39729,7 @@
       </c>
       <c r="AV184" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW184" s="20" t="inlineStr">
@@ -40153,7 +40153,7 @@
       </c>
       <c r="AV186" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW186" s="20" t="inlineStr">
@@ -40388,7 +40388,7 @@
       </c>
       <c r="AZ187" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA187" s="20" t="inlineStr">
@@ -40592,7 +40592,7 @@
       </c>
       <c r="AV188" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW188" s="20" t="inlineStr">
@@ -40827,7 +40827,7 @@
       </c>
       <c r="AZ189" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA189" s="20" t="inlineStr">
@@ -41039,7 +41039,7 @@
       </c>
       <c r="AZ190" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA190" s="20" t="inlineStr">
@@ -41430,7 +41430,7 @@
       </c>
       <c r="AR192" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS192" s="20" t="inlineStr">
@@ -41652,7 +41652,7 @@
       </c>
       <c r="AR193" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS193" s="20" t="inlineStr">
@@ -42288,7 +42288,7 @@
       </c>
       <c r="AQ196" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AR196" s="20" t="inlineStr">
@@ -42987,7 +42987,7 @@
       </c>
       <c r="AZ199" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="BA199" s="20" t="inlineStr">
@@ -43171,7 +43171,7 @@
       </c>
       <c r="AR200" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AS200" s="20" t="inlineStr">
@@ -43388,7 +43388,7 @@
       </c>
       <c r="AR201" s="20" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="AS201" s="20" t="inlineStr">
@@ -43408,7 +43408,7 @@
       </c>
       <c r="AV201" s="20" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="AW201" s="20" t="inlineStr">

</xml_diff>